<commit_message>
Went back to old tilemap
</commit_message>
<xml_diff>
--- a/Course Notes.xlsx
+++ b/Course Notes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38360" windowHeight="17710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38360" windowHeight="17710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Game Outline" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>http://netcell.github.io/phaser-inspector/</t>
   </si>
@@ -67,16 +67,60 @@
   </si>
   <si>
     <t>Intro</t>
+  </si>
+  <si>
+    <t>https://www.codeandweb.com/texturepacker/tutorials/creating-spritesheets-for-phaser-with-texturepacker</t>
+  </si>
+  <si>
+    <t>Texture Packer</t>
+  </si>
+  <si>
+    <t>http://mightyfingers.com/</t>
+  </si>
+  <si>
+    <t>Phaser framework/editor</t>
+  </si>
+  <si>
+    <t>https://vimeo.com/album/3156158</t>
+  </si>
+  <si>
+    <t>mightyfingers videos</t>
+  </si>
+  <si>
+    <t>http://inkubator.io/inkubatethis.html</t>
+  </si>
+  <si>
+    <t>mightyfingers blog</t>
+  </si>
+  <si>
+    <t>https://elmvids.groob.io/</t>
+  </si>
+  <si>
+    <t>Elm Videos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZwaomOYGuYo</t>
+  </si>
+  <si>
+    <t>Tile video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,13 +143,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -494,15 +541,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="1" max="1" width="61.36328125" customWidth="1"/>
     <col min="2" max="2" width="53.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,7 +561,58 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>